<commit_message>
Add MKB and NKB Reflectivity
</commit_message>
<xml_diff>
--- a/data/hom_refl/B4C_refl.xlsx
+++ b/data/hom_refl/B4C_refl.xlsx
@@ -29,6 +29,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -112,13 +113,13 @@
   </sheetPr>
   <dimension ref="A1:O501"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A478" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P501" activeCellId="0" sqref="P501"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.54"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="21.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="0" width="12.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.68"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="7" style="0" width="12.83"/>

</xml_diff>